<commit_message>
finalized the setup, introduced trimming down to 500 and some comments
</commit_message>
<xml_diff>
--- a/GeoJSON-tracks-simplified-Circle.xlsx
+++ b/GeoJSON-tracks-simplified-Circle.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D541"/>
+  <dimension ref="A1:D501"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9455,726 +9455,6 @@
         <v>174</v>
       </c>
     </row>
-    <row r="502">
-      <c r="A502" s="1" t="n">
-        <v>500</v>
-      </c>
-      <c r="B502" t="inlineStr">
-        <is>
-          <t>Solbråtan</t>
-        </is>
-      </c>
-      <c r="C502" t="inlineStr">
-        <is>
-          <t>{"type": "Feature", "geometry": {"type": "Point", "coordinates": [10.804319584783196, 59.8016790922524]}, "properties": {"Navn": "Solbråtan", "subType": "Circle", "radius": 100}}</t>
-        </is>
-      </c>
-      <c r="D502" t="n">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="503">
-      <c r="A503" s="1" t="n">
-        <v>501</v>
-      </c>
-      <c r="B503" t="inlineStr">
-        <is>
-          <t>Bondivann</t>
-        </is>
-      </c>
-      <c r="C503" t="inlineStr">
-        <is>
-          <t>{"type": "Feature", "geometry": {"type": "Point", "coordinates": [10.4329129635055, 59.82062824961597]}, "properties": {"Navn": "Bondivann", "subType": "Circle", "radius": 100}}</t>
-        </is>
-      </c>
-      <c r="D503" t="n">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="504">
-      <c r="A504" s="1" t="n">
-        <v>502</v>
-      </c>
-      <c r="B504" t="inlineStr">
-        <is>
-          <t>Hamar</t>
-        </is>
-      </c>
-      <c r="C504" t="inlineStr">
-        <is>
-          <t>{"type": "Feature", "geometry": {"type": "Point", "coordinates": [11.07702095516146, 60.79139691461184]}, "properties": {"Navn": "Hamar", "subType": "Circle", "radius": 100}}</t>
-        </is>
-      </c>
-      <c r="D504" t="n">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="505">
-      <c r="A505" s="1" t="n">
-        <v>503</v>
-      </c>
-      <c r="B505" t="inlineStr">
-        <is>
-          <t>Reinunga</t>
-        </is>
-      </c>
-      <c r="C505" t="inlineStr">
-        <is>
-          <t>{"type": "Feature", "geometry": {"type": "Point", "coordinates": [7.138568132360481, 60.74407159531161]}, "properties": {"Navn": "Reinunga", "subType": "Circle", "radius": 100}}</t>
-        </is>
-      </c>
-      <c r="D505" t="n">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="506">
-      <c r="A506" s="1" t="n">
-        <v>504</v>
-      </c>
-      <c r="B506" t="inlineStr">
-        <is>
-          <t>Ogna</t>
-        </is>
-      </c>
-      <c r="C506" t="inlineStr">
-        <is>
-          <t>{"type": "Feature", "geometry": {"type": "Point", "coordinates": [5.803277542370785, 58.519698680005085]}, "properties": {"Navn": "Ogna", "subType": "Circle", "radius": 100}}</t>
-        </is>
-      </c>
-      <c r="D506" t="n">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="507">
-      <c r="A507" s="1" t="n">
-        <v>505</v>
-      </c>
-      <c r="B507" t="inlineStr">
-        <is>
-          <t>Notodden kollektivterminal</t>
-        </is>
-      </c>
-      <c r="C507" t="inlineStr">
-        <is>
-          <t>{"type": "Feature", "geometry": {"type": "Point", "coordinates": [9.257170867052322, 59.55704708955216]}, "properties": {"Navn": "Notodden kollektivterminal", "subType": "Circle", "radius": 100}}</t>
-        </is>
-      </c>
-      <c r="D507" t="n">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="508">
-      <c r="A508" s="1" t="n">
-        <v>506</v>
-      </c>
-      <c r="B508" t="inlineStr">
-        <is>
-          <t>Stod</t>
-        </is>
-      </c>
-      <c r="C508" t="inlineStr">
-        <is>
-          <t>{"type": "Feature", "geometry": {"type": "Point", "coordinates": [11.733839754830653, 64.12011876533623]}, "properties": {"Navn": "Stod", "subType": "Circle", "radius": 100}}</t>
-        </is>
-      </c>
-      <c r="D508" t="n">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="509">
-      <c r="A509" s="1" t="n">
-        <v>507</v>
-      </c>
-      <c r="B509" t="inlineStr">
-        <is>
-          <t>Vevelstad</t>
-        </is>
-      </c>
-      <c r="C509" t="inlineStr">
-        <is>
-          <t>{"type": "Feature", "geometry": {"type": "Point", "coordinates": [10.837419506843142, 59.75626687843042]}, "properties": {"Navn": "Vevelstad", "subType": "Circle", "radius": 100}}</t>
-        </is>
-      </c>
-      <c r="D509" t="n">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="510">
-      <c r="A510" s="1" t="n">
-        <v>508</v>
-      </c>
-      <c r="B510" t="inlineStr">
-        <is>
-          <t>Hallingskeid</t>
-        </is>
-      </c>
-      <c r="C510" t="inlineStr">
-        <is>
-          <t>{"type": "Feature", "geometry": {"type": "Point", "coordinates": [7.252311118838984, 60.66801173514526]}, "properties": {"Navn": "Hallingskeid", "subType": "Circle", "radius": 100}}</t>
-        </is>
-      </c>
-      <c r="D510" t="n">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="511">
-      <c r="A511" s="1" t="n">
-        <v>509</v>
-      </c>
-      <c r="B511" t="inlineStr">
-        <is>
-          <t>Nærbø</t>
-        </is>
-      </c>
-      <c r="C511" t="inlineStr">
-        <is>
-          <t>{"type": "Feature", "geometry": {"type": "Point", "coordinates": [5.640261662529382, 58.66548879864698]}, "properties": {"Navn": "Nærbø", "subType": "Circle", "radius": 100}}</t>
-        </is>
-      </c>
-      <c r="D511" t="n">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="512">
-      <c r="A512" s="1" t="n">
-        <v>510</v>
-      </c>
-      <c r="B512" t="inlineStr">
-        <is>
-          <t>Meheia</t>
-        </is>
-      </c>
-      <c r="C512" t="inlineStr">
-        <is>
-          <t>{"type": "Feature", "geometry": {"type": "Point", "coordinates": [9.500967453148784, 59.63013433952929]}, "properties": {"Navn": "Meheia", "subType": "Circle", "radius": 100}}</t>
-        </is>
-      </c>
-      <c r="D512" t="n">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="513">
-      <c r="A513" s="1" t="n">
-        <v>511</v>
-      </c>
-      <c r="B513" t="inlineStr">
-        <is>
-          <t>Galterud</t>
-        </is>
-      </c>
-      <c r="C513" t="inlineStr">
-        <is>
-          <t>{"type": "Feature", "geometry": {"type": "Point", "coordinates": [11.88106109873164, 60.19721943061114]}, "properties": {"Navn": "Galterud", "subType": "Circle", "radius": 100}}</t>
-        </is>
-      </c>
-      <c r="D513" t="n">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="514">
-      <c r="A514" s="1" t="n">
-        <v>512</v>
-      </c>
-      <c r="B514" t="inlineStr">
-        <is>
-          <t>Nisterud</t>
-        </is>
-      </c>
-      <c r="C514" t="inlineStr">
-        <is>
-          <t>{"type": "Feature", "geometry": {"type": "Point", "coordinates": [9.485111821605479, 59.30039047603001]}, "properties": {"Navn": "Nisterud", "subType": "Circle", "radius": 100}}</t>
-        </is>
-      </c>
-      <c r="D514" t="n">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="515">
-      <c r="A515" s="1" t="n">
-        <v>513</v>
-      </c>
-      <c r="B515" t="inlineStr">
-        <is>
-          <t>Blommenholm</t>
-        </is>
-      </c>
-      <c r="C515" t="inlineStr">
-        <is>
-          <t>{"type": "Feature", "geometry": {"type": "Point", "coordinates": [10.555019697856967, 59.897324665626705]}, "properties": {"Navn": "Blommenholm", "subType": "Circle", "radius": 100}}</t>
-        </is>
-      </c>
-      <c r="D515" t="n">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="516">
-      <c r="A516" s="1" t="n">
-        <v>514</v>
-      </c>
-      <c r="B516" t="inlineStr">
-        <is>
-          <t>Drivstua</t>
-        </is>
-      </c>
-      <c r="C516" t="inlineStr">
-        <is>
-          <t>{"type": "Feature", "geometry": {"type": "Point", "coordinates": [9.625158106611305, 62.424409689109616]}, "properties": {"Navn": "Drivstua", "subType": "Circle", "radius": 100}}</t>
-        </is>
-      </c>
-      <c r="D516" t="n">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="517">
-      <c r="A517" s="1" t="n">
-        <v>515</v>
-      </c>
-      <c r="B517" t="inlineStr">
-        <is>
-          <t>Hauerseter</t>
-        </is>
-      </c>
-      <c r="C517" t="inlineStr">
-        <is>
-          <t>{"type": "Feature", "geometry": {"type": "Point", "coordinates": [11.195037446245353, 60.185331340700124]}, "properties": {"Navn": "Hauerseter", "subType": "Circle", "radius": 100}}</t>
-        </is>
-      </c>
-      <c r="D517" t="n">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="518">
-      <c r="A518" s="1" t="n">
-        <v>516</v>
-      </c>
-      <c r="B518" t="inlineStr">
-        <is>
-          <t>Bjorli</t>
-        </is>
-      </c>
-      <c r="C518" t="inlineStr">
-        <is>
-          <t>{"type": "Feature", "geometry": {"type": "Point", "coordinates": [8.201509418533021, 62.25835394385295]}, "properties": {"Navn": "Bjorli", "subType": "Circle", "radius": 100}}</t>
-        </is>
-      </c>
-      <c r="D518" t="n">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="519">
-      <c r="A519" s="1" t="n">
-        <v>517</v>
-      </c>
-      <c r="B519" t="inlineStr">
-        <is>
-          <t>Atna</t>
-        </is>
-      </c>
-      <c r="C519" t="inlineStr">
-        <is>
-          <t>{"type": "Feature", "geometry": {"type": "Point", "coordinates": [10.834817545787839, 61.732516414224804]}, "properties": {"Navn": "Atna", "subType": "Circle", "radius": 100}}</t>
-        </is>
-      </c>
-      <c r="D519" t="n">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="520">
-      <c r="A520" s="1" t="n">
-        <v>518</v>
-      </c>
-      <c r="B520" t="inlineStr">
-        <is>
-          <t>Ørtfjell</t>
-        </is>
-      </c>
-      <c r="C520" t="inlineStr">
-        <is>
-          <t>{"type": "Feature", "geometry": {"type": "Point", "coordinates": [14.69862360253075, 66.39898425540288]}, "properties": {"Navn": "Ørtfjell", "subType": "Circle", "radius": 100}}</t>
-        </is>
-      </c>
-      <c r="D520" t="n">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="521">
-      <c r="A521" s="1" t="n">
-        <v>519</v>
-      </c>
-      <c r="B521" t="inlineStr">
-        <is>
-          <t>Trolldalen</t>
-        </is>
-      </c>
-      <c r="C521" t="inlineStr">
-        <is>
-          <t>{"type": "Feature", "geometry": {"type": "Point", "coordinates": [9.683358389532081, 60.30299053592365]}, "properties": {"Navn": "Trolldalen", "subType": "Circle", "radius": 100}}</t>
-        </is>
-      </c>
-      <c r="D521" t="n">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="522">
-      <c r="A522" s="1" t="n">
-        <v>520</v>
-      </c>
-      <c r="B522" t="inlineStr">
-        <is>
-          <t>Ingedal</t>
-        </is>
-      </c>
-      <c r="C522" t="inlineStr">
-        <is>
-          <t>{"type": "Feature", "geometry": {"type": "Point", "coordinates": [11.239559686962922, 59.158666056763884]}, "properties": {"Navn": "Ingedal", "subType": "Circle", "radius": 100}}</t>
-        </is>
-      </c>
-      <c r="D522" t="n">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="523">
-      <c r="A523" s="1" t="n">
-        <v>521</v>
-      </c>
-      <c r="B523" t="inlineStr">
-        <is>
-          <t>Bleiken</t>
-        </is>
-      </c>
-      <c r="C523" t="inlineStr">
-        <is>
-          <t>{"type": "Feature", "geometry": {"type": "Point", "coordinates": [10.500566837079583, 60.4687242570112]}, "properties": {"Navn": "Bleiken", "subType": "Circle", "radius": 100}}</t>
-        </is>
-      </c>
-      <c r="D523" t="n">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="524">
-      <c r="A524" s="1" t="n">
-        <v>522</v>
-      </c>
-      <c r="B524" t="inlineStr">
-        <is>
-          <t>Dale</t>
-        </is>
-      </c>
-      <c r="C524" t="inlineStr">
-        <is>
-          <t>{"type": "Feature", "geometry": {"type": "Point", "coordinates": [5.816092603216047, 60.586276954062555]}, "properties": {"Navn": "Dale", "subType": "Circle", "radius": 100}}</t>
-        </is>
-      </c>
-      <c r="D524" t="n">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="525">
-      <c r="A525" s="1" t="n">
-        <v>523</v>
-      </c>
-      <c r="B525" t="inlineStr">
-        <is>
-          <t>Bergsgrav</t>
-        </is>
-      </c>
-      <c r="C525" t="inlineStr">
-        <is>
-          <t>{"type": "Feature", "geometry": {"type": "Point", "coordinates": [11.471325395642344, 63.771322986147304]}, "properties": {"Navn": "Bergsgrav", "subType": "Circle", "radius": 100}}</t>
-        </is>
-      </c>
-      <c r="D525" t="n">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="526">
-      <c r="A526" s="1" t="n">
-        <v>524</v>
-      </c>
-      <c r="B526" t="inlineStr">
-        <is>
-          <t>Ljan</t>
-        </is>
-      </c>
-      <c r="C526" t="inlineStr">
-        <is>
-          <t>{"type": "Feature", "geometry": {"type": "Point", "coordinates": [10.78476771347253, 59.85329621560522]}, "properties": {"Navn": "Ljan", "subType": "Circle", "radius": 100}}</t>
-        </is>
-      </c>
-      <c r="D526" t="n">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="527">
-      <c r="A527" s="1" t="n">
-        <v>525</v>
-      </c>
-      <c r="B527" t="inlineStr">
-        <is>
-          <t>Tangen</t>
-        </is>
-      </c>
-      <c r="C527" t="inlineStr">
-        <is>
-          <t>{"type": "Feature", "geometry": {"type": "Point", "coordinates": [11.269986926434944, 60.6159012605446]}, "properties": {"Navn": "Tangen", "subType": "Circle", "radius": 100}}</t>
-        </is>
-      </c>
-      <c r="D527" t="n">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="528">
-      <c r="A528" s="1" t="n">
-        <v>526</v>
-      </c>
-      <c r="B528" t="inlineStr">
-        <is>
-          <t>Ualand</t>
-        </is>
-      </c>
-      <c r="C528" t="inlineStr">
-        <is>
-          <t>{"type": "Feature", "geometry": {"type": "Point", "coordinates": [6.3432723357129275, 58.5286870937457]}, "properties": {"Navn": "Ualand", "subType": "Circle", "radius": 100}}</t>
-        </is>
-      </c>
-      <c r="D528" t="n">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="529">
-      <c r="A529" s="1" t="n">
-        <v>527</v>
-      </c>
-      <c r="B529" t="inlineStr">
-        <is>
-          <t>Ustaoset</t>
-        </is>
-      </c>
-      <c r="C529" t="inlineStr">
-        <is>
-          <t>{"type": "Feature", "geometry": {"type": "Point", "coordinates": [8.045120280866234, 60.4964326595444]}, "properties": {"Navn": "Ustaoset", "subType": "Circle", "radius": 100}}</t>
-        </is>
-      </c>
-      <c r="D529" t="n">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="530">
-      <c r="A530" s="1" t="n">
-        <v>528</v>
-      </c>
-      <c r="B530" t="inlineStr">
-        <is>
-          <t>Mjøndalen</t>
-        </is>
-      </c>
-      <c r="C530" t="inlineStr">
-        <is>
-          <t>{"type": "Feature", "geometry": {"type": "Point", "coordinates": [10.011501929479081, 59.75101806652755]}, "properties": {"Navn": "Mjøndalen", "subType": "Circle", "radius": 100}}</t>
-        </is>
-      </c>
-      <c r="D530" t="n">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="531">
-      <c r="A531" s="1" t="n">
-        <v>529</v>
-      </c>
-      <c r="B531" t="inlineStr">
-        <is>
-          <t>Nypan</t>
-        </is>
-      </c>
-      <c r="C531" t="inlineStr">
-        <is>
-          <t>{"type": "Feature", "geometry": {"type": "Point", "coordinates": [10.336913269418693, 63.31658831454024]}, "properties": {"Navn": "Nypan", "subType": "Circle", "radius": 100}}</t>
-        </is>
-      </c>
-      <c r="D531" t="n">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="532">
-      <c r="A532" s="1" t="n">
-        <v>530</v>
-      </c>
-      <c r="B532" t="inlineStr">
-        <is>
-          <t>Eidsberg</t>
-        </is>
-      </c>
-      <c r="C532" t="inlineStr">
-        <is>
-          <t>{"type": "Feature", "geometry": {"type": "Point", "coordinates": [11.303594894127583, 59.513427503355906]}, "properties": {"Navn": "Eidsberg", "subType": "Circle", "radius": 100}}</t>
-        </is>
-      </c>
-      <c r="D532" t="n">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="533">
-      <c r="A533" s="1" t="n">
-        <v>531</v>
-      </c>
-      <c r="B533" t="inlineStr">
-        <is>
-          <t>Sjoa</t>
-        </is>
-      </c>
-      <c r="C533" t="inlineStr">
-        <is>
-          <t>{"type": "Feature", "geometry": {"type": "Point", "coordinates": [9.541729021958322, 61.68238466164242]}, "properties": {"Navn": "Sjoa", "subType": "Circle", "radius": 100}}</t>
-        </is>
-      </c>
-      <c r="D533" t="n">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="534">
-      <c r="A534" s="1" t="n">
-        <v>532</v>
-      </c>
-      <c r="B534" t="inlineStr">
-        <is>
-          <t>Fjellhamar</t>
-        </is>
-      </c>
-      <c r="C534" t="inlineStr">
-        <is>
-          <t>{"type": "Feature", "geometry": {"type": "Point", "coordinates": [10.981828838928449, 59.94064332846252]}, "properties": {"Navn": "Fjellhamar", "subType": "Circle", "radius": 100}}</t>
-        </is>
-      </c>
-      <c r="D534" t="n">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="535">
-      <c r="A535" s="1" t="n">
-        <v>533</v>
-      </c>
-      <c r="B535" t="inlineStr">
-        <is>
-          <t>Djupvik</t>
-        </is>
-      </c>
-      <c r="C535" t="inlineStr">
-        <is>
-          <t>{"type": "Feature", "geometry": {"type": "Point", "coordinates": [17.543832058107903, 68.44887035373951]}, "properties": {"Navn": "Djupvik", "subType": "Circle", "radius": 100}}</t>
-        </is>
-      </c>
-      <c r="D535" t="n">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="536">
-      <c r="A536" s="1" t="n">
-        <v>534</v>
-      </c>
-      <c r="B536" t="inlineStr">
-        <is>
-          <t>Boganes</t>
-        </is>
-      </c>
-      <c r="C536" t="inlineStr">
-        <is>
-          <t>{"type": "Feature", "geometry": {"type": "Point", "coordinates": [5.73631261996474, 58.90688910728376]}, "properties": {"Navn": "Boganes", "subType": "Circle", "radius": 100}}</t>
-        </is>
-      </c>
-      <c r="D536" t="n">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="537">
-      <c r="A537" s="1" t="n">
-        <v>535</v>
-      </c>
-      <c r="B537" t="inlineStr">
-        <is>
-          <t>Orstad</t>
-        </is>
-      </c>
-      <c r="C537" t="inlineStr">
-        <is>
-          <t>{"type": "Feature", "geometry": {"type": "Point", "coordinates": [5.705291780204769, 58.7992729226776]}, "properties": {"Navn": "Orstad", "subType": "Circle", "radius": 100}}</t>
-        </is>
-      </c>
-      <c r="D537" t="n">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="538">
-      <c r="A538" s="1" t="n">
-        <v>536</v>
-      </c>
-      <c r="B538" t="inlineStr">
-        <is>
-          <t>Martineåsen</t>
-        </is>
-      </c>
-      <c r="C538" t="inlineStr">
-        <is>
-          <t>{"type": "Feature", "geometry": {"type": "Point", "coordinates": [9.971176459487252, 59.05985708452194]}, "properties": {"Navn": "Martineåsen", "subType": "Circle", "radius": 100}}</t>
-        </is>
-      </c>
-      <c r="D538" t="n">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="539">
-      <c r="A539" s="1" t="n">
-        <v>537</v>
-      </c>
-      <c r="B539" t="inlineStr">
-        <is>
-          <t>Hobekk</t>
-        </is>
-      </c>
-      <c r="C539" t="inlineStr">
-        <is>
-          <t>{"type": "Feature", "geometry": {"type": "Point", "coordinates": [9.900835621590202, 59.07039884292061]}, "properties": {"Navn": "Hobekk", "subType": "Circle", "radius": 100}}</t>
-        </is>
-      </c>
-      <c r="D539" t="n">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="540">
-      <c r="A540" s="1" t="n">
-        <v>538</v>
-      </c>
-      <c r="B540" t="inlineStr">
-        <is>
-          <t>Myrane</t>
-        </is>
-      </c>
-      <c r="C540" t="inlineStr">
-        <is>
-          <t>{"type": "Feature", "geometry": {"type": "Point", "coordinates": [9.676942873601533, 59.126980977819976]}, "properties": {"Navn": "Myrane", "subType": "Circle", "radius": 100}}</t>
-        </is>
-      </c>
-      <c r="D540" t="n">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="541">
-      <c r="A541" s="1" t="n">
-        <v>539</v>
-      </c>
-      <c r="B541" t="inlineStr">
-        <is>
-          <t>Ørvik</t>
-        </is>
-      </c>
-      <c r="C541" t="inlineStr">
-        <is>
-          <t>{"type": "Feature", "geometry": {"type": "Point", "coordinates": [9.688286504556736, 59.07225719471918]}, "properties": {"Navn": "Ørvik", "subType": "Circle", "radius": 100}}</t>
-        </is>
-      </c>
-      <c r="D541" t="n">
-        <v>174</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>